<commit_message>
begin to add beam pipe"
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-Gauss-Gabor.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-Gauss-Gabor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE6080B-2618-FF42-B668-643CB1DED69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025BF21-60DC-6147-AF86-DE0C9534B2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11740" yWindow="640" windowWidth="18500" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="68">
   <si>
     <t>Parameter</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>Drift to next Gabor lens</t>
+  </si>
+  <si>
+    <t>Vacuum chamber</t>
+  </si>
+  <si>
+    <t>Mother volume radius</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -471,6 +477,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,52 +862,52 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="16">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="17">
         <v>15</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -912,17 +922,15 @@
       <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>15</v>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -939,7 +947,7 @@
         <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2">
         <v>3.9999999999999998E-6</v>
@@ -948,7 +956,7 @@
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -965,16 +973,16 @@
         <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2">
-        <v>15</v>
+        <v>3.9999999999999998E-6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -991,90 +999,90 @@
         <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="2">
-        <v>0.3</v>
+        <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>0.998</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="8">
         <v>0.05</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1085,69 +1093,72 @@
         <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2">
         <v>0.05</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F14" s="3">
         <v>2.8700000000000002E-3</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>1</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1158,22 +1169,19 @@
         <v>34</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="10">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1190,40 +1198,43 @@
         <v>35</v>
       </c>
       <c r="E16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>1</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <f>2.4916949087545</f>
         <v>2.4916949087544999</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
-        <v>1</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17">
-        <v>0.15</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1246,7 +1257,7 @@
         <v>14</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1257,22 +1268,19 @@
         <v>34</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F19">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1289,88 +1297,90 @@
         <v>35</v>
       </c>
       <c r="E20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>1</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>1.0187472612650501</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="11">
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="11">
         <v>0.15</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="7" t="s">
+      <c r="G22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
-        <v>1</v>
-      </c>
-      <c r="B22" s="9" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>1</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="9">
+      <c r="C23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="9">
         <v>0.5</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="9" t="s">
+      <c r="G23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
-        <v>1</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1381,21 +1391,21 @@
         <v>39</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>35</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D24" s="10"/>
       <c r="E24" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="10">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="10"/>
+      <c r="H24" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
@@ -1411,13 +1421,13 @@
         <v>35</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F25" s="10">
-        <v>1.4485646330252</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="H25" s="10"/>
     </row>
@@ -1429,21 +1439,21 @@
         <v>39</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="10"/>
+        <v>62</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="E26" s="10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F26" s="10">
-        <v>0.15</v>
+        <v>1.4485646330252</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
@@ -1460,13 +1470,13 @@
         <v>18</v>
       </c>
       <c r="F27" s="10">
-        <v>1.7709999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1484,13 +1494,13 @@
         <v>18</v>
       </c>
       <c r="F28" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>1.7709999999999999</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1501,22 +1511,20 @@
         <v>39</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D29" s="10"/>
       <c r="E29" s="10" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F29" s="10">
-        <v>2.5000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1527,20 +1535,22 @@
         <v>39</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="E30" s="10" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F30" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1558,12 +1568,14 @@
         <v>18</v>
       </c>
       <c r="F31" s="10">
-        <v>6.4610000000000001E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="10"/>
+      <c r="H31" s="10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
@@ -1580,7 +1592,7 @@
         <v>18</v>
       </c>
       <c r="F32" s="10">
-        <v>0.13539000000000001</v>
+        <v>6.4610000000000001E-2</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>14</v>
@@ -1602,14 +1614,12 @@
         <v>18</v>
       </c>
       <c r="F33" s="10">
-        <v>0.01</v>
+        <v>0.13539000000000001</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
@@ -1626,84 +1636,84 @@
         <v>18</v>
       </c>
       <c r="F34" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="10">
         <v>5.4600000000000003E-2</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>1</v>
-      </c>
-      <c r="B35" s="7" t="s">
+      <c r="G35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="7">
+      <c r="C36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="7">
         <v>0.5</v>
       </c>
-      <c r="G35" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="7" t="s">
+      <c r="G36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="9">
-        <v>1</v>
-      </c>
-      <c r="B36" s="9" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>1</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="9">
+      <c r="C37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="9">
         <v>0.15</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="9" t="s">
+      <c r="G37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="10">
-        <v>1</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="10">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="10">
@@ -1719,13 +1729,13 @@
         <v>35</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38">
-        <v>1.7888589662779599</v>
+        <v>18</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0.85699999999999998</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="H38" s="13"/>
     </row>
@@ -1737,20 +1747,21 @@
         <v>45</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>17</v>
+        <v>62</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F39">
-        <v>0.15</v>
+        <v>1.7888589662779599</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
@@ -1766,12 +1777,14 @@
         <v>18</v>
       </c>
       <c r="F40">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="G40" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="13"/>
+      <c r="H40" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
@@ -1787,14 +1800,12 @@
         <v>18</v>
       </c>
       <c r="F41">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
@@ -1804,21 +1815,20 @@
         <v>45</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F42">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="13"/>
+      <c r="H42" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="10">
@@ -1834,13 +1844,13 @@
         <v>35</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F43">
-        <v>1.60433994066042</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="H43" s="13"/>
     </row>
@@ -1852,20 +1862,21 @@
         <v>45</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>17</v>
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
+        <v>35</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F44">
-        <v>0.15</v>
+        <v>1.60433994066042</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
@@ -1881,12 +1892,14 @@
         <v>18</v>
       </c>
       <c r="F45">
-        <v>2.5</v>
+        <v>0.15</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="13"/>
+      <c r="H45" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
@@ -1902,14 +1915,12 @@
         <v>18</v>
       </c>
       <c r="F46">
-        <v>0.15</v>
+        <v>2.5</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="10">
@@ -1919,21 +1930,20 @@
         <v>45</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F47">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="13"/>
+      <c r="H47" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
@@ -1949,13 +1959,13 @@
         <v>35</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F48">
-        <v>1.2448140165275099</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="H48" s="13"/>
     </row>
@@ -1967,20 +1977,21 @@
         <v>45</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>17</v>
+        <v>62</v>
+      </c>
+      <c r="D49" t="s">
+        <v>35</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F49">
-        <v>0.15</v>
+        <v>1.2448140165275099</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H49" s="13"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="10">
@@ -1996,12 +2007,14 @@
         <v>18</v>
       </c>
       <c r="F50">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="13"/>
+      <c r="H50" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="10">
@@ -2017,14 +2030,12 @@
         <v>18</v>
       </c>
       <c r="F51">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="10">
@@ -2034,21 +2045,20 @@
         <v>45</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F52">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="13"/>
+      <c r="H52" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="10">
@@ -2064,61 +2074,63 @@
         <v>35</v>
       </c>
       <c r="E53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="10">
+        <v>1</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>1.1659674896013299</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G54" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H53" s="13"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>1</v>
-      </c>
-      <c r="B54" s="7" t="s">
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>1</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" s="11">
+      <c r="C55" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="11"/>
+      <c r="E55" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="11">
         <v>0.15</v>
       </c>
-      <c r="G54" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H54" s="7" t="s">
+      <c r="G55" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="10">
-        <v>1</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F55" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
@@ -2128,16 +2140,14 @@
         <v>52</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D56" s="10"/>
       <c r="E56" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F56" s="10">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>14</v>
@@ -2158,13 +2168,13 @@
         <v>54</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="F57" s="10">
-        <v>45</v>
+        <v>0.8</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="H57" s="10"/>
     </row>
@@ -2176,17 +2186,19 @@
         <v>52</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="E58" s="10" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="F58" s="10">
-        <v>0.2</v>
+        <v>45</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="H58" s="10"/>
     </row>
@@ -2198,21 +2210,21 @@
         <v>52</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D59" s="10"/>
       <c r="E59" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F59" s="10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H59" s="10"/>
     </row>
-    <row r="60" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="10">
         <v>1</v>
       </c>
@@ -2224,17 +2236,17 @@
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F60" s="10">
-        <v>22.544</v>
+        <v>0.1</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>1</v>
       </c>
@@ -2242,17 +2254,17 @@
         <v>52</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F61" s="10">
-        <v>0.4</v>
+        <v>22.544</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H61" s="10"/>
     </row>
@@ -2264,21 +2276,21 @@
         <v>52</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F62" s="10">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H62" s="10"/>
     </row>
-    <row r="63" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="10">
         <v>1</v>
       </c>
@@ -2290,17 +2302,17 @@
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F63" s="10">
-        <v>31.376799999999999</v>
+        <v>0.1</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="H63" s="10"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A64" s="10">
         <v>1</v>
       </c>
@@ -2308,17 +2320,17 @@
         <v>52</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F64" s="10">
-        <v>0.2</v>
+        <v>31.376799999999999</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H64" s="10"/>
     </row>
@@ -2330,21 +2342,21 @@
         <v>52</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F65" s="10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="10"/>
     </row>
-    <row r="66" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="10">
         <v>1</v>
       </c>
@@ -2356,17 +2368,17 @@
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F66" s="10">
-        <v>31.5123</v>
+        <v>0.1</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="H66" s="10"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A67" s="10">
         <v>1</v>
       </c>
@@ -2374,38 +2386,38 @@
         <v>52</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F67" s="10">
+        <v>31.5123</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="10">
+        <v>1</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="10">
         <f>0.2-0.005</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="G67" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H67" s="10"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="10">
-        <v>1</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="10">
-        <v>0.01</v>
-      </c>
       <c r="G68" s="10" t="s">
         <v>14</v>
       </c>
@@ -2426,37 +2438,37 @@
         <v>18</v>
       </c>
       <c r="F69" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="10">
+        <v>1</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="10">
         <f>0.2-0.005</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="G69" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H69" s="10"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="10">
-        <v>1</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="10">
-        <v>0.1</v>
-      </c>
       <c r="G70" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="10">
         <v>1</v>
       </c>
@@ -2468,18 +2480,17 @@
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F71" s="10">
-        <f>F66</f>
-        <v>31.5123</v>
+        <v>0.1</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A72" s="10">
         <v>1</v>
       </c>
@@ -2487,17 +2498,18 @@
         <v>52</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F72" s="10">
-        <v>0.2</v>
+        <f>F67</f>
+        <v>31.5123</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H72" s="10"/>
     </row>
@@ -2509,21 +2521,21 @@
         <v>52</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D73" s="10"/>
       <c r="E73" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F73" s="10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H73" s="10"/>
     </row>
-    <row r="74" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>1</v>
       </c>
@@ -2535,18 +2547,17 @@
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F74" s="10">
-        <f>F63</f>
-        <v>31.376799999999999</v>
+        <v>0.1</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
         <v>1</v>
       </c>
@@ -2554,17 +2565,18 @@
         <v>52</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D75" s="10"/>
       <c r="E75" s="10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F75" s="10">
-        <v>0.4</v>
+        <f>F64</f>
+        <v>31.376799999999999</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H75" s="10"/>
     </row>
@@ -2576,21 +2588,21 @@
         <v>52</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D76" s="10"/>
       <c r="E76" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F76" s="10">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="G76" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H76" s="10"/>
     </row>
-    <row r="77" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>1</v>
       </c>
@@ -2602,18 +2614,17 @@
       </c>
       <c r="D77" s="10"/>
       <c r="E77" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F77" s="10">
-        <f>F60</f>
-        <v>22.544</v>
+        <v>0.1</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
         <v>1</v>
       </c>
@@ -2621,17 +2632,18 @@
         <v>52</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D78" s="10"/>
       <c r="E78" s="10" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F78" s="10">
-        <v>0.2</v>
+        <f>F61</f>
+        <v>22.544</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H78" s="10"/>
     </row>
@@ -2643,16 +2655,14 @@
         <v>52</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D79" s="10"/>
       <c r="E79" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F79" s="10">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>14</v>
@@ -2673,13 +2683,13 @@
         <v>54</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="F80" s="10">
-        <v>45</v>
+        <v>0.8</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="H80" s="10"/>
     </row>
@@ -2691,41 +2701,65 @@
         <v>52</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D81" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="E81" s="10" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="F81" s="10">
+        <v>45</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="10">
+        <v>1</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F82" s="10">
         <v>0.2</v>
       </c>
-      <c r="G81" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H81" s="10"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="7">
-        <v>1</v>
-      </c>
-      <c r="B82" s="7" t="s">
+      <c r="G82" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="7">
+        <v>1</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C82" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F82" s="7">
+      <c r="C83" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83" s="7">
         <v>2</v>
       </c>
-      <c r="G82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H82" s="7"/>
+      <c r="G83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H83" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Gabor fix up for carbon
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-Gauss-Gabor.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-Gauss-Gabor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2020294991307/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E62442-445B-7447-A828-770A9FFF3B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{68E62442-445B-7447-A828-770A9FFF3B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0800B75E-AC43-D941-B5D7-3F26923DA17A}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="640" windowWidth="18500" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>